<commit_message>
open source tool for creating forms
</commit_message>
<xml_diff>
--- a/Coke Scholars Virtual Visitas (Responses).xlsx
+++ b/Coke Scholars Virtual Visitas (Responses).xlsx
@@ -1,52 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alber\OneDrive - Georgia Institute of Technology\GitHub\VirtualVisitas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF7B9F0-7C74-46D4-9AE9-5172C2B5C182}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="C31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment authorId="0" ref="C31">
       <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Responder updated this value.</t>
-        </r>
+        <t xml:space="preserve">Responder updated this value.</t>
       </text>
     </comment>
-    <comment ref="K31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment authorId="0" ref="K31">
       <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Responder updated this value.</t>
-        </r>
+        <t xml:space="preserve">Responder updated this value.</t>
       </text>
     </comment>
   </commentList>
@@ -54,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="248">
   <si>
     <t>Timestamp</t>
   </si>
@@ -783,77 +760,87 @@
   </si>
   <si>
     <t>Music, Theater, Reading, Shopping, Research, Debate</t>
+  </si>
+  <si>
+    <t>albertzhang9000@gmail.com</t>
+  </si>
+  <si>
+    <t>Albert Zhang</t>
+  </si>
+  <si>
+    <t>Rap, Classical, EDM</t>
+  </si>
+  <si>
+    <t>Swimming &amp; Diving, Cross Country, Track and Field</t>
+  </si>
+  <si>
+    <t>Cooking/Baking, Research, Debate, Volunteering</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1043,29 +1030,26 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="20" width="21.5703125" customWidth="1"/>
+    <col customWidth="1" min="1" max="20" width="21.57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1109,7 +1093,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="2">
         <v>43907.57072909722</v>
       </c>
@@ -1141,9 +1125,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="2">
-        <v>43907.571418888889</v>
+        <v>43907.57141888889</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>23</v>
@@ -1185,9 +1169,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="2">
-        <v>43907.571655624997</v>
+        <v>43907.571655625</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>35</v>
@@ -1220,9 +1204,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5">
       <c r="A5" s="2">
-        <v>43907.571664490737</v>
+        <v>43907.57166449074</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>43</v>
@@ -1252,9 +1236,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6">
       <c r="A6" s="2">
-        <v>43907.573801643521</v>
+        <v>43907.57380164352</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>50</v>
@@ -1284,9 +1268,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7">
       <c r="A7" s="2">
-        <v>43907.576695532407</v>
+        <v>43907.57669553241</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>56</v>
@@ -1322,7 +1306,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8">
       <c r="A8" s="2">
         <v>43907.580455625</v>
       </c>
@@ -1357,7 +1341,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9">
       <c r="A9" s="2">
         <v>43907.589197430556</v>
       </c>
@@ -1392,9 +1376,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10">
       <c r="A10" s="2">
-        <v>43907.593132465277</v>
+        <v>43907.59313246528</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>80</v>
@@ -1430,7 +1414,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11">
       <c r="A11" s="2">
         <v>43907.593966053246</v>
       </c>
@@ -1471,9 +1455,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12">
       <c r="A12" s="2">
-        <v>43907.603203240738</v>
+        <v>43907.60320324074</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>99</v>
@@ -1506,7 +1490,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13">
       <c r="A13" s="2">
         <v>43907.608694803246</v>
       </c>
@@ -1538,9 +1522,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14">
       <c r="A14" s="2">
-        <v>43907.612164594902</v>
+        <v>43907.6121645949</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>114</v>
@@ -1573,7 +1557,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15">
       <c r="A15" s="2">
         <v>43907.61463398148</v>
       </c>
@@ -1605,7 +1589,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16">
       <c r="A16" s="2">
         <v>43907.616207569445</v>
       </c>
@@ -1637,9 +1621,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17">
       <c r="A17" s="2">
-        <v>43907.616223263889</v>
+        <v>43907.61622326389</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>133</v>
@@ -1669,9 +1653,9 @@
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18">
       <c r="A18" s="2">
-        <v>43907.621333842588</v>
+        <v>43907.62133384259</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>140</v>
@@ -1704,7 +1688,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19">
       <c r="A19" s="2">
         <v>43907.658861944445</v>
       </c>
@@ -1736,7 +1720,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20">
       <c r="A20" s="2">
         <v>43907.69471851852</v>
       </c>
@@ -1768,9 +1752,9 @@
         <v>159</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21">
       <c r="A21" s="2">
-        <v>43907.697456238428</v>
+        <v>43907.69745623843</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>160</v>
@@ -1800,9 +1784,9 @@
         <v>163</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22">
       <c r="A22" s="2">
-        <v>43907.740139131944</v>
+        <v>43907.74013913194</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>164</v>
@@ -1841,7 +1825,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23">
       <c r="A23" s="2">
         <v>43907.7924546875</v>
       </c>
@@ -1873,9 +1857,9 @@
         <v>177</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24">
       <c r="A24" s="2">
-        <v>43907.844439166671</v>
+        <v>43907.84443916667</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>178</v>
@@ -1914,9 +1898,9 @@
         <v>185</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25">
       <c r="A25" s="2">
-        <v>43907.946862500001</v>
+        <v>43907.9468625</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>186</v>
@@ -1946,7 +1930,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26">
       <c r="A26" s="2">
         <v>43908.430335578705</v>
       </c>
@@ -1981,9 +1965,9 @@
         <v>198</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27">
       <c r="A27" s="2">
-        <v>43908.680709780092</v>
+        <v>43908.68070978009</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>199</v>
@@ -2013,9 +1997,9 @@
         <v>205</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28">
       <c r="A28" s="2">
-        <v>43908.682651909723</v>
+        <v>43908.68265190972</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>206</v>
@@ -2045,7 +2029,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29">
       <c r="A29" s="2">
         <v>43908.689684791665</v>
       </c>
@@ -2077,9 +2061,9 @@
         <v>218</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30">
       <c r="A30" s="2">
-        <v>43908.718877893523</v>
+        <v>43908.71887789352</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>219</v>
@@ -2112,7 +2096,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31">
       <c r="A31" s="5">
         <v>43908.784570902775</v>
       </c>
@@ -2147,9 +2131,9 @@
         <v>235</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32">
       <c r="A32" s="2">
-        <v>43908.795496099541</v>
+        <v>43908.79549609954</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>236</v>
@@ -2179,8 +2163,40 @@
         <v>242</v>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" s="2">
+        <v>43908.8344866088</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
rq groups manual small big
</commit_message>
<xml_diff>
--- a/Coke Scholars Virtual Visitas (Responses).xlsx
+++ b/Coke Scholars Virtual Visitas (Responses).xlsx
@@ -31,6 +31,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Responder updated this value.</t>
         </r>
@@ -43,6 +44,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Responder updated this value.</t>
         </r>
@@ -53,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="247">
   <si>
     <t>Timestamp</t>
   </si>
@@ -94,9 +96,6 @@
     <t>Texas</t>
   </si>
   <si>
-    <t>Art, Film, and Visual Studies, Theater, Dance, and Media</t>
-  </si>
-  <si>
     <t>Pop, Kpop</t>
   </si>
   <si>
@@ -151,9 +150,6 @@
     <t>Illinois</t>
   </si>
   <si>
-    <t>Government, Human Developmental and Regenerative Biology, Women, Gender, and Sexuality, Studies of</t>
-  </si>
-  <si>
     <t>Pop, Rap, R&amp;B, EDM, Kpop</t>
   </si>
   <si>
@@ -262,9 +258,6 @@
     <t>Nevada</t>
   </si>
   <si>
-    <t>Government, Women, Gender, and Sexuality, Studies of</t>
-  </si>
-  <si>
     <t>Pop, Rap, R&amp;B, Indie</t>
   </si>
   <si>
@@ -700,9 +693,6 @@
     <t>Anisha Holla</t>
   </si>
   <si>
-    <t>Prefrosh (if you're class of 2024)</t>
-  </si>
-  <si>
     <t>Chemical and Physical Biology</t>
   </si>
   <si>
@@ -730,9 +720,6 @@
     <t>Arkansas</t>
   </si>
   <si>
-    <t>Sociology, Women, Gender, and Sexuality, Studies of</t>
-  </si>
-  <si>
     <t>Pop, Rap, R&amp;B, Alternative</t>
   </si>
   <si>
@@ -797,6 +784,18 @@
   </si>
   <si>
     <t>Grade</t>
+  </si>
+  <si>
+    <t>Art Film and Visual Studies, Theater Dance and Media</t>
+  </si>
+  <si>
+    <t>Government, Human Developmental and Regenerative Biology, Studies of Women Gender and Sexuality</t>
+  </si>
+  <si>
+    <t>Government, Studies of Women Gender and Sexuality</t>
+  </si>
+  <si>
+    <t>Sociology, Studies of Women Gender and Sexuality</t>
   </si>
 </sst>
 </file>
@@ -806,7 +805,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -816,10 +815,18 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1071,7 +1078,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1093,22 +1100,22 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -1143,16 +1150,16 @@
         <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1160,43 +1167,43 @@
         <v>43907.571418888889</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1204,34 +1211,34 @@
         <v>43907.571655624997</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1239,31 +1246,31 @@
         <v>43907.571664490737</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1271,31 +1278,31 @@
         <v>43907.573801643521</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1303,37 +1310,37 @@
         <v>43907.576695532407</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1341,34 +1348,34 @@
         <v>43907.580455625</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1376,34 +1383,34 @@
         <v>43907.589197430556</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="G9" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1411,37 +1418,37 @@
         <v>43907.593132465277</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="K10" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="L10" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1449,40 +1456,40 @@
         <v>43907.593966053246</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="J11" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="K11" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="M11" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="N11" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1490,34 +1497,34 @@
         <v>43907.603203240738</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="H12" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="J12" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="K12" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1525,31 +1532,31 @@
         <v>43907.608694803246</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="J13" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1557,34 +1564,34 @@
         <v>43907.612164594902</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="3" t="s">
+      <c r="I14" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="J14" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="L14" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1592,31 +1599,31 @@
         <v>43907.61463398148</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="I15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1624,31 +1631,31 @@
         <v>43907.616207569445</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="I16" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G16" s="3" t="s">
+      <c r="J16" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1656,31 +1663,31 @@
         <v>43907.616223263889</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="J17" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1688,34 +1695,34 @@
         <v>43907.621333842588</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="3" t="s">
+      <c r="I18" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="J18" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="K18" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1723,31 +1730,31 @@
         <v>43907.658861944445</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="I19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1755,31 +1762,31 @@
         <v>43907.69471851852</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="3" t="s">
+      <c r="I20" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="J20" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1787,31 +1794,31 @@
         <v>43907.697456238428</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="J21" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1819,40 +1826,40 @@
         <v>43907.740139131944</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I22" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="M22" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="N22" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1860,31 +1867,31 @@
         <v>43907.7924546875</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="H23" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="3" t="s">
+      <c r="I23" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="J23" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1892,40 +1899,40 @@
         <v>43907.844439166671</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="3" t="s">
+      <c r="I24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G24" s="3" t="s">
+      <c r="L24" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="M24" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="I24" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J24" s="3" t="s">
+      <c r="N24" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="M24" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1933,31 +1940,31 @@
         <v>43907.946862500001</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="3" t="s">
+      <c r="I25" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="J25" s="3" t="s">
         <v>182</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1965,34 +1972,34 @@
         <v>43908.430335578705</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="3" t="s">
+      <c r="I26" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G26" s="3" t="s">
+      <c r="J26" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="K26" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2000,31 +2007,31 @@
         <v>43908.680709780092</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="3" t="s">
+      <c r="H27" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F27" s="3" t="s">
+      <c r="I27" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="J27" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="12.3" x14ac:dyDescent="0.4">
@@ -2032,31 +2039,31 @@
         <v>43908.682651909723</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="H28" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="3" t="s">
+      <c r="I28" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="J28" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="12.3" x14ac:dyDescent="0.4">
@@ -2064,31 +2071,31 @@
         <v>43908.689684791665</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="H29" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="3" t="s">
+      <c r="I29" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" s="3" t="s">
+      <c r="J29" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="12.3" x14ac:dyDescent="0.4">
@@ -2096,34 +2103,34 @@
         <v>43908.718877893523</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>215</v>
+        <v>18</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G30" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="M30" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="M30" s="3" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="12.3" x14ac:dyDescent="0.4">
@@ -2131,34 +2138,34 @@
         <v>43908.784570902775</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="H31" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="I31" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="J31" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="F31" s="3" t="s">
+      <c r="K31" s="3" t="s">
         <v>224</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="J31" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="K31" s="3" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="12.3" x14ac:dyDescent="0.4">
@@ -2166,31 +2173,31 @@
         <v>43908.795496099541</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="I32" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="3" t="s">
+      <c r="J32" s="3" t="s">
         <v>231</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
@@ -2198,31 +2205,31 @@
         <v>43908.834486608801</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>215</v>
+        <v>18</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reverted back to a working main_friday. I don't think any other files were affected.
</commit_message>
<xml_diff>
--- a/Coke Scholars Virtual Visitas (Responses).xlsx
+++ b/Coke Scholars Virtual Visitas (Responses).xlsx
@@ -31,7 +31,6 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
           </rPr>
           <t>Responder updated this value.</t>
         </r>
@@ -44,7 +43,6 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
-            <family val="2"/>
           </rPr>
           <t>Responder updated this value.</t>
         </r>
@@ -55,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="248">
   <si>
     <t>Timestamp</t>
   </si>
@@ -96,6 +94,9 @@
     <t>Texas</t>
   </si>
   <si>
+    <t>Art, Film, and Visual Studies, Theater, Dance, and Media</t>
+  </si>
+  <si>
     <t>Pop, Kpop</t>
   </si>
   <si>
@@ -150,6 +151,9 @@
     <t>Illinois</t>
   </si>
   <si>
+    <t>Government, Human Developmental and Regenerative Biology, Women, Gender, and Sexuality, Studies of</t>
+  </si>
+  <si>
     <t>Pop, Rap, R&amp;B, EDM, Kpop</t>
   </si>
   <si>
@@ -258,6 +262,9 @@
     <t>Nevada</t>
   </si>
   <si>
+    <t>Government, Women, Gender, and Sexuality, Studies of</t>
+  </si>
+  <si>
     <t>Pop, Rap, R&amp;B, Indie</t>
   </si>
   <si>
@@ -693,6 +700,9 @@
     <t>Anisha Holla</t>
   </si>
   <si>
+    <t>Prefrosh (if you're class of 2024)</t>
+  </si>
+  <si>
     <t>Chemical and Physical Biology</t>
   </si>
   <si>
@@ -720,6 +730,9 @@
     <t>Arkansas</t>
   </si>
   <si>
+    <t>Sociology, Women, Gender, and Sexuality, Studies of</t>
+  </si>
+  <si>
     <t>Pop, Rap, R&amp;B, Alternative</t>
   </si>
   <si>
@@ -784,18 +797,6 @@
   </si>
   <si>
     <t>Grade</t>
-  </si>
-  <si>
-    <t>Art Film and Visual Studies, Theater Dance and Media</t>
-  </si>
-  <si>
-    <t>Government, Human Developmental and Regenerative Biology, Studies of Women Gender and Sexuality</t>
-  </si>
-  <si>
-    <t>Government, Studies of Women Gender and Sexuality</t>
-  </si>
-  <si>
-    <t>Sociology, Studies of Women Gender and Sexuality</t>
   </si>
 </sst>
 </file>
@@ -805,7 +806,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -815,18 +816,10 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1078,7 +1071,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1100,22 +1093,22 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>237</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -1150,16 +1143,16 @@
         <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>243</v>
+        <v>13</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1167,43 +1160,43 @@
         <v>43907.571418888889</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1211,34 +1204,34 @@
         <v>43907.571655624997</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>244</v>
+        <v>32</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1246,31 +1239,31 @@
         <v>43907.571664490737</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1278,31 +1271,31 @@
         <v>43907.573801643521</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1310,37 +1303,37 @@
         <v>43907.576695532407</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1348,34 +1341,34 @@
         <v>43907.580455625</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1383,34 +1376,34 @@
         <v>43907.589197430556</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>245</v>
+        <v>69</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1418,37 +1411,37 @@
         <v>43907.593132465277</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1456,40 +1449,40 @@
         <v>43907.593966053246</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1497,34 +1490,34 @@
         <v>43907.603203240738</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1532,31 +1525,31 @@
         <v>43907.608694803246</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1564,34 +1557,34 @@
         <v>43907.612164594902</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1599,31 +1592,31 @@
         <v>43907.61463398148</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1631,31 +1624,31 @@
         <v>43907.616207569445</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1663,31 +1656,31 @@
         <v>43907.616223263889</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1695,34 +1688,34 @@
         <v>43907.621333842588</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1730,31 +1723,31 @@
         <v>43907.658861944445</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1762,31 +1755,31 @@
         <v>43907.69471851852</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1794,31 +1787,31 @@
         <v>43907.697456238428</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1826,40 +1819,40 @@
         <v>43907.740139131944</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1867,31 +1860,31 @@
         <v>43907.7924546875</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1899,40 +1892,40 @@
         <v>43907.844439166671</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1940,31 +1933,31 @@
         <v>43907.946862500001</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1972,34 +1965,34 @@
         <v>43908.430335578705</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -2007,31 +2000,31 @@
         <v>43908.680709780092</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="12.3" x14ac:dyDescent="0.4">
@@ -2039,31 +2032,31 @@
         <v>43908.682651909723</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="12.3" x14ac:dyDescent="0.4">
@@ -2071,31 +2064,31 @@
         <v>43908.689684791665</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="12.3" x14ac:dyDescent="0.4">
@@ -2103,34 +2096,34 @@
         <v>43908.718877893523</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="12.3" x14ac:dyDescent="0.4">
@@ -2138,34 +2131,34 @@
         <v>43908.784570902775</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="12.3" x14ac:dyDescent="0.4">
@@ -2173,31 +2166,31 @@
         <v>43908.795496099541</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="12.3" x14ac:dyDescent="0.4">
@@ -2205,31 +2198,31 @@
         <v>43908.834486608801</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>